<commit_message>
wireframes and updated task list
</commit_message>
<xml_diff>
--- a/docs/task-list.xlsx
+++ b/docs/task-list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8250"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8250" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mobile" sheetId="1" r:id="rId1"/>
@@ -531,7 +531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -694,7 +694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
changes to task list
</commit_message>
<xml_diff>
--- a/docs/task-list.xlsx
+++ b/docs/task-list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="65">
   <si>
     <t>Sr No</t>
   </si>
@@ -102,15 +102,9 @@
     <t>Techno-digital Profile</t>
   </si>
   <si>
-    <t>History page</t>
-  </si>
-  <si>
     <t>Logic to update campaign page</t>
   </si>
   <si>
-    <t>Settings page</t>
-  </si>
-  <si>
     <t>Mobile Framework with project</t>
   </si>
   <si>
@@ -178,6 +172,45 @@
   </si>
   <si>
     <t>API for profile details POST</t>
+  </si>
+  <si>
+    <t>Richa</t>
+  </si>
+  <si>
+    <t>Sadhvi</t>
+  </si>
+  <si>
+    <t>Login Page</t>
+  </si>
+  <si>
+    <t>Nitin</t>
+  </si>
+  <si>
+    <t>Keshav</t>
+  </si>
+  <si>
+    <t>Megha</t>
+  </si>
+  <si>
+    <t>Eric</t>
+  </si>
+  <si>
+    <t>Pranav</t>
+  </si>
+  <si>
+    <t>Jobs Page</t>
+  </si>
+  <si>
+    <t>timeline page</t>
+  </si>
+  <si>
+    <t>Sync page</t>
+  </si>
+  <si>
+    <t>Jobs Details</t>
+  </si>
+  <si>
+    <t>My Referals</t>
   </si>
 </sst>
 </file>
@@ -529,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,7 +599,7 @@
         <v>42585</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -580,7 +613,7 @@
         <v>42646</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -588,7 +621,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1">
         <v>42677</v>
@@ -610,13 +643,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1">
         <v>42677</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -629,6 +662,9 @@
       <c r="C7" t="s">
         <v>14</v>
       </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -640,16 +676,22 @@
       <c r="C8" t="s">
         <v>14</v>
       </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -657,10 +699,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -668,10 +713,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -679,10 +727,52 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -692,10 +782,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,7 +821,7 @@
         <v>42585</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -745,7 +835,7 @@
         <v>42646</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -759,10 +849,10 @@
         <v>42646</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -776,10 +866,10 @@
         <v>42677</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -793,10 +883,10 @@
         <v>42707</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -810,7 +900,7 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -823,6 +913,9 @@
       <c r="C8" t="s">
         <v>14</v>
       </c>
+      <c r="E8" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -834,16 +927,22 @@
       <c r="C9" t="s">
         <v>14</v>
       </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -857,7 +956,7 @@
         <v>42646</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -865,13 +964,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1">
         <v>42646</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -879,10 +978,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -890,10 +992,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -901,10 +1006,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -912,10 +1020,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -939,6 +1050,9 @@
       <c r="C18" s="1">
         <v>42707</v>
       </c>
+      <c r="E18" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -1000,7 +1114,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
@@ -1011,16 +1125,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C25" s="1">
         <v>42707</v>
       </c>
       <c r="D25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1028,16 +1142,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C26" s="1">
         <v>42707</v>
       </c>
       <c r="D26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1045,7 +1159,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
         <v>14</v>
@@ -1056,7 +1170,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="E28" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1064,7 +1181,18 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>51</v>
+      </c>
+      <c r="E29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1113,7 +1241,7 @@
         <v>42554</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1127,7 +1255,7 @@
         <v>42585</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>